<commit_message>
First data lectures, small fixes
</commit_message>
<xml_diff>
--- a/2 - Data Load, clean, and save/data/RAS200.xlsx
+++ b/2 - Data Load, clean, and save/data/RAS200.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
   <x:si>
     <x:t>Activity and employment rates (end November) by frequency, sex, age, ancestry, region and time</x:t>
   </x:si>
@@ -61,13 +61,16 @@
     <x:t>2020</x:t>
   </x:si>
   <x:si>
+    <x:t>2021</x:t>
+  </x:si>
+  <x:si>
     <x:t>Employment rate</x:t>
   </x:si>
   <x:si>
     <x:t>Total</x:t>
   </x:si>
   <x:si>
-    <x:t>16-64 years total</x:t>
+    <x:t>16-64 years</x:t>
   </x:si>
   <x:si>
     <x:t>All Denmark</x:t>
@@ -818,7 +821,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:R119"/>
+  <x:dimension ref="A1:S119"/>
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0"/>
   </x:sheetViews>
@@ -826,23 +829,23 @@
   <x:cols>
     <x:col min="1" max="1" width="18.270625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="7.270625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.410625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="12.840625000000001" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="7.270625" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="28.550625" style="0" customWidth="1"/>
-    <x:col min="6" max="18" width="6.980625" style="0" customWidth="1"/>
+    <x:col min="6" max="19" width="6.980625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:18">
+    <x:row r="1" spans="1:19">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:18">
+    <x:row r="2" spans="1:19">
       <x:c r="A2" s="2" t="s">
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:18">
+    <x:row r="3" spans="1:19">
       <x:c r="F3" s="3" t="s">
         <x:v>2</x:v>
       </x:c>
@@ -882,22 +885,25 @@
       <x:c r="R3" s="3" t="s">
         <x:v>14</x:v>
       </x:c>
-    </x:row>
-    <x:row r="4" spans="1:18">
+      <x:c r="S3" s="3" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:19">
       <x:c r="A4" s="3" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B4" s="3" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C4" s="3" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D4" s="3" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="D4" s="3" t="s">
-        <x:v>16</x:v>
-      </x:c>
       <x:c r="E4" s="3" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="F4" s="4" t="n">
         <x:v>76</x:v>
@@ -938,10 +944,13 @@
       <x:c r="R4" s="4" t="n">
         <x:v>74.5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="5" spans="1:18">
+      <x:c r="S4" s="4" t="n">
+        <x:v>77.1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:19">
       <x:c r="E5" s="3" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F5" s="4" t="n">
         <x:v>75.8</x:v>
@@ -982,10 +991,13 @@
       <x:c r="R5" s="4" t="n">
         <x:v>75</x:v>
       </x:c>
-    </x:row>
-    <x:row r="6" spans="1:18">
+      <x:c r="S5" s="4" t="n">
+        <x:v>77.7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:19">
       <x:c r="E6" s="3" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F6" s="4" t="n">
         <x:v>73.4</x:v>
@@ -1026,10 +1038,13 @@
       <x:c r="R6" s="4" t="n">
         <x:v>73.6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="7" spans="1:18">
+      <x:c r="S6" s="4" t="n">
+        <x:v>76.7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:19">
       <x:c r="E7" s="3" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F7" s="4" t="n">
         <x:v>72.5</x:v>
@@ -1070,10 +1085,13 @@
       <x:c r="R7" s="4" t="n">
         <x:v>72.8</x:v>
       </x:c>
-    </x:row>
-    <x:row r="8" spans="1:18">
+      <x:c r="S7" s="4" t="n">
+        <x:v>76.1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:19">
       <x:c r="E8" s="3" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="F8" s="4" t="n">
         <x:v>75.6</x:v>
@@ -1114,10 +1132,13 @@
       <x:c r="R8" s="4" t="n">
         <x:v>76.6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="9" spans="1:18">
+      <x:c r="S8" s="4" t="n">
+        <x:v>79.1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:19">
       <x:c r="E9" s="3" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F9" s="4" t="n">
         <x:v>80.5</x:v>
@@ -1158,10 +1179,13 @@
       <x:c r="R9" s="4" t="n">
         <x:v>80.4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="10" spans="1:18">
+      <x:c r="S9" s="4" t="n">
+        <x:v>82.3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:19">
       <x:c r="E10" s="3" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="F10" s="4" t="n">
         <x:v>79</x:v>
@@ -1202,10 +1226,13 @@
       <x:c r="R10" s="4" t="n">
         <x:v>77.5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="11" spans="1:18">
+      <x:c r="S10" s="4" t="n">
+        <x:v>79.7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:19">
       <x:c r="E11" s="3" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F11" s="4" t="n">
         <x:v>77.1</x:v>
@@ -1246,10 +1273,13 @@
       <x:c r="R11" s="4" t="n">
         <x:v>74.9</x:v>
       </x:c>
-    </x:row>
-    <x:row r="12" spans="1:18">
+      <x:c r="S11" s="4" t="n">
+        <x:v>77.4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:19">
       <x:c r="E12" s="3" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F12" s="4" t="n">
         <x:v>73.1</x:v>
@@ -1290,10 +1320,13 @@
       <x:c r="R12" s="4" t="n">
         <x:v>70.8</x:v>
       </x:c>
-    </x:row>
-    <x:row r="13" spans="1:18">
+      <x:c r="S12" s="4" t="n">
+        <x:v>73.6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:19">
       <x:c r="E13" s="3" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="F13" s="4" t="n">
         <x:v>75.9</x:v>
@@ -1334,10 +1367,13 @@
       <x:c r="R13" s="4" t="n">
         <x:v>74.7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="14" spans="1:18">
+      <x:c r="S13" s="4" t="n">
+        <x:v>77</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:19">
       <x:c r="E14" s="3" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F14" s="4" t="n">
         <x:v>72.3</x:v>
@@ -1378,10 +1414,13 @@
       <x:c r="R14" s="4" t="n">
         <x:v>69.5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="15" spans="1:18">
+      <x:c r="S14" s="4" t="n">
+        <x:v>73.2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:19">
       <x:c r="E15" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="F15" s="4" t="n">
         <x:v>79.2</x:v>
@@ -1422,10 +1461,13 @@
       <x:c r="R15" s="4" t="n">
         <x:v>76.1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="16" spans="1:18">
+      <x:c r="S15" s="4" t="n">
+        <x:v>78.2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:19">
       <x:c r="E16" s="3" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F16" s="4" t="n">
         <x:v>77.9</x:v>
@@ -1466,10 +1508,13 @@
       <x:c r="R16" s="4" t="n">
         <x:v>76.6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="17" spans="1:18">
+      <x:c r="S16" s="4" t="n">
+        <x:v>79.1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:19">
       <x:c r="E17" s="3" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F17" s="4" t="n">
         <x:v>79.2</x:v>
@@ -1510,10 +1555,13 @@
       <x:c r="R17" s="4" t="n">
         <x:v>76.6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="18" spans="1:18">
+      <x:c r="S17" s="4" t="n">
+        <x:v>78.8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:19">
       <x:c r="E18" s="3" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="F18" s="4" t="n">
         <x:v>77.7</x:v>
@@ -1554,10 +1602,13 @@
       <x:c r="R18" s="4" t="n">
         <x:v>76.4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="19" spans="1:18">
+      <x:c r="S18" s="4" t="n">
+        <x:v>78.9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:19">
       <x:c r="E19" s="3" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="F19" s="4" t="n">
         <x:v>78</x:v>
@@ -1598,10 +1649,13 @@
       <x:c r="R19" s="4" t="n">
         <x:v>75.2</x:v>
       </x:c>
-    </x:row>
-    <x:row r="20" spans="1:18">
+      <x:c r="S19" s="4" t="n">
+        <x:v>77.7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:19">
       <x:c r="E20" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F20" s="4" t="n">
         <x:v>76.5</x:v>
@@ -1642,10 +1696,13 @@
       <x:c r="R20" s="4" t="n">
         <x:v>74.4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="21" spans="1:18">
+      <x:c r="S20" s="4" t="n">
+        <x:v>77</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:19">
       <x:c r="E21" s="3" t="s">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="F21" s="4" t="n">
         <x:v>72.8</x:v>
@@ -1686,10 +1743,13 @@
       <x:c r="R21" s="4" t="n">
         <x:v>70.9</x:v>
       </x:c>
-    </x:row>
-    <x:row r="22" spans="1:18">
+      <x:c r="S21" s="4" t="n">
+        <x:v>73.7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:19">
       <x:c r="E22" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="F22" s="4" t="n">
         <x:v>78.7</x:v>
@@ -1730,10 +1790,13 @@
       <x:c r="R22" s="4" t="n">
         <x:v>75.3</x:v>
       </x:c>
-    </x:row>
-    <x:row r="23" spans="1:18">
+      <x:c r="S22" s="4" t="n">
+        <x:v>77.1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:19">
       <x:c r="E23" s="3" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="F23" s="4" t="n">
         <x:v>78</x:v>
@@ -1774,10 +1837,13 @@
       <x:c r="R23" s="4" t="n">
         <x:v>75.7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="24" spans="1:18">
+      <x:c r="S23" s="4" t="n">
+        <x:v>79</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:19">
       <x:c r="E24" s="3" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="F24" s="4" t="n">
         <x:v>82.4</x:v>
@@ -1818,10 +1884,13 @@
       <x:c r="R24" s="4" t="n">
         <x:v>80.1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="25" spans="1:18">
+      <x:c r="S24" s="4" t="n">
+        <x:v>82.1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:19">
       <x:c r="E25" s="3" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F25" s="4" t="n">
         <x:v>79.4</x:v>
@@ -1862,10 +1931,13 @@
       <x:c r="R25" s="4" t="n">
         <x:v>78.4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="26" spans="1:18">
+      <x:c r="S25" s="4" t="n">
+        <x:v>80.4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:19">
       <x:c r="E26" s="3" t="s">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="F26" s="4" t="n">
         <x:v>83.8</x:v>
@@ -1906,10 +1978,13 @@
       <x:c r="R26" s="4" t="n">
         <x:v>82.6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="27" spans="1:18">
+      <x:c r="S26" s="4" t="n">
+        <x:v>84.3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:19">
       <x:c r="E27" s="3" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="F27" s="4" t="n">
         <x:v>84</x:v>
@@ -1950,10 +2025,13 @@
       <x:c r="R27" s="4" t="n">
         <x:v>82.7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="28" spans="1:18">
+      <x:c r="S27" s="4" t="n">
+        <x:v>84.2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:19">
       <x:c r="E28" s="3" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F28" s="4" t="n">
         <x:v>78.1</x:v>
@@ -1994,10 +2072,13 @@
       <x:c r="R28" s="4" t="n">
         <x:v>77</x:v>
       </x:c>
-    </x:row>
-    <x:row r="29" spans="1:18">
+      <x:c r="S28" s="4" t="n">
+        <x:v>79.4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:19">
       <x:c r="E29" s="3" t="s">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="F29" s="4" t="n">
         <x:v>79.9</x:v>
@@ -2038,10 +2119,13 @@
       <x:c r="R29" s="4" t="n">
         <x:v>78.2</x:v>
       </x:c>
-    </x:row>
-    <x:row r="30" spans="1:18">
+      <x:c r="S29" s="4" t="n">
+        <x:v>80.1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:19">
       <x:c r="E30" s="3" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="F30" s="4" t="n">
         <x:v>80.5</x:v>
@@ -2082,10 +2166,13 @@
       <x:c r="R30" s="4" t="n">
         <x:v>80</x:v>
       </x:c>
-    </x:row>
-    <x:row r="31" spans="1:18">
+      <x:c r="S30" s="4" t="n">
+        <x:v>81.9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:19">
       <x:c r="E31" s="3" t="s">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F31" s="4" t="n">
         <x:v>78</x:v>
@@ -2126,10 +2213,13 @@
       <x:c r="R31" s="4" t="n">
         <x:v>77.6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="32" spans="1:18">
+      <x:c r="S31" s="4" t="n">
+        <x:v>79.3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:19">
       <x:c r="E32" s="3" t="s">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="F32" s="4" t="n">
         <x:v>75.8</x:v>
@@ -2170,10 +2260,13 @@
       <x:c r="R32" s="4" t="n">
         <x:v>75.6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="33" spans="1:18">
+      <x:c r="S32" s="4" t="n">
+        <x:v>77.3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:19">
       <x:c r="E33" s="3" t="s">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="F33" s="4" t="n">
         <x:v>75.9</x:v>
@@ -2214,10 +2307,13 @@
       <x:c r="R33" s="4" t="n">
         <x:v>75.4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="34" spans="1:18">
+      <x:c r="S33" s="4" t="n">
+        <x:v>78</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:19">
       <x:c r="E34" s="3" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="F34" s="4" t="n">
         <x:v>81.4</x:v>
@@ -2258,10 +2354,13 @@
       <x:c r="R34" s="4" t="n">
         <x:v>78.9</x:v>
       </x:c>
-    </x:row>
-    <x:row r="35" spans="1:18">
+      <x:c r="S34" s="4" t="n">
+        <x:v>80.8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:19">
       <x:c r="E35" s="3" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F35" s="4" t="n">
         <x:v>80.1</x:v>
@@ -2302,10 +2401,13 @@
       <x:c r="R35" s="4" t="n">
         <x:v>78.9</x:v>
       </x:c>
-    </x:row>
-    <x:row r="36" spans="1:18">
+      <x:c r="S35" s="4" t="n">
+        <x:v>81</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:19">
       <x:c r="E36" s="3" t="s">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="F36" s="4" t="n">
         <x:v>79</x:v>
@@ -2346,10 +2448,13 @@
       <x:c r="R36" s="4" t="n">
         <x:v>77.7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="37" spans="1:18">
+      <x:c r="S36" s="4" t="n">
+        <x:v>79.9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:19">
       <x:c r="E37" s="3" t="s">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="F37" s="4" t="n">
         <x:v>68</x:v>
@@ -2390,10 +2495,13 @@
       <x:c r="R37" s="4" t="n">
         <x:v>70.3</x:v>
       </x:c>
-    </x:row>
-    <x:row r="38" spans="1:18">
+      <x:c r="S37" s="4" t="n">
+        <x:v>73.8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:19">
       <x:c r="E38" s="3" t="s">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F38" s="4" t="n">
         <x:v>68</x:v>
@@ -2434,10 +2542,13 @@
       <x:c r="R38" s="4" t="n">
         <x:v>70.3</x:v>
       </x:c>
-    </x:row>
-    <x:row r="39" spans="1:18">
+      <x:c r="S38" s="4" t="n">
+        <x:v>73.7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:19">
       <x:c r="E39" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="F39" s="4" t="n">
         <x:v>62.9</x:v>
@@ -2478,10 +2589,13 @@
       <x:c r="R39" s="4" t="n">
         <x:v>79.2</x:v>
       </x:c>
-    </x:row>
-    <x:row r="40" spans="1:18">
+      <x:c r="S39" s="4" t="n">
+        <x:v>76</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:19">
       <x:c r="E40" s="3" t="s">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="F40" s="4" t="n">
         <x:v>75.7</x:v>
@@ -2522,10 +2636,13 @@
       <x:c r="R40" s="4" t="n">
         <x:v>74.7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="41" spans="1:18">
+      <x:c r="S40" s="4" t="n">
+        <x:v>76.9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:19">
       <x:c r="E41" s="3" t="s">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="F41" s="4" t="n">
         <x:v>79.5</x:v>
@@ -2566,10 +2683,13 @@
       <x:c r="R41" s="4" t="n">
         <x:v>78.3</x:v>
       </x:c>
-    </x:row>
-    <x:row r="42" spans="1:18">
+      <x:c r="S41" s="4" t="n">
+        <x:v>80.4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:19">
       <x:c r="E42" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="F42" s="4" t="n">
         <x:v>79.6</x:v>
@@ -2610,10 +2730,13 @@
       <x:c r="R42" s="4" t="n">
         <x:v>79.1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="43" spans="1:18">
+      <x:c r="S42" s="4" t="n">
+        <x:v>81.1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:19">
       <x:c r="E43" s="3" t="s">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="F43" s="4" t="n">
         <x:v>78.4</x:v>
@@ -2654,10 +2777,13 @@
       <x:c r="R43" s="4" t="n">
         <x:v>76.8</x:v>
       </x:c>
-    </x:row>
-    <x:row r="44" spans="1:18">
+      <x:c r="S43" s="4" t="n">
+        <x:v>78.8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:19">
       <x:c r="E44" s="3" t="s">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="F44" s="4" t="n">
         <x:v>81.5</x:v>
@@ -2698,10 +2824,13 @@
       <x:c r="R44" s="4" t="n">
         <x:v>79.7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="45" spans="1:18">
+      <x:c r="S44" s="4" t="n">
+        <x:v>81.6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:19">
       <x:c r="E45" s="3" t="s">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="F45" s="4" t="n">
         <x:v>79.1</x:v>
@@ -2742,10 +2871,13 @@
       <x:c r="R45" s="4" t="n">
         <x:v>77.6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="46" spans="1:18">
+      <x:c r="S45" s="4" t="n">
+        <x:v>79.8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:19">
       <x:c r="E46" s="3" t="s">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="F46" s="4" t="n">
         <x:v>81.8</x:v>
@@ -2786,10 +2918,13 @@
       <x:c r="R46" s="4" t="n">
         <x:v>81.8</x:v>
       </x:c>
-    </x:row>
-    <x:row r="47" spans="1:18">
+      <x:c r="S46" s="4" t="n">
+        <x:v>83.9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:19">
       <x:c r="E47" s="3" t="s">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="F47" s="4" t="n">
         <x:v>74.2</x:v>
@@ -2830,10 +2965,13 @@
       <x:c r="R47" s="4" t="n">
         <x:v>73.1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="48" spans="1:18">
+      <x:c r="S47" s="4" t="n">
+        <x:v>75.4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:19">
       <x:c r="E48" s="3" t="s">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="F48" s="4" t="n">
         <x:v>77.8</x:v>
@@ -2874,10 +3012,13 @@
       <x:c r="R48" s="4" t="n">
         <x:v>76.5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="49" spans="1:18">
+      <x:c r="S48" s="4" t="n">
+        <x:v>78.3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:19">
       <x:c r="E49" s="3" t="s">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="F49" s="4" t="n">
         <x:v>71.7</x:v>
@@ -2918,10 +3059,13 @@
       <x:c r="R49" s="4" t="n">
         <x:v>70.5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="50" spans="1:18">
+      <x:c r="S49" s="4" t="n">
+        <x:v>73.2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:19">
       <x:c r="E50" s="3" t="s">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="F50" s="4" t="n">
         <x:v>76.7</x:v>
@@ -2962,10 +3106,13 @@
       <x:c r="R50" s="4" t="n">
         <x:v>75.5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="51" spans="1:18">
+      <x:c r="S50" s="4" t="n">
+        <x:v>78</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:19">
       <x:c r="E51" s="3" t="s">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="F51" s="4" t="n">
         <x:v>74.2</x:v>
@@ -3006,10 +3153,13 @@
       <x:c r="R51" s="4" t="n">
         <x:v>71.6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="52" spans="1:18">
+      <x:c r="S51" s="4" t="n">
+        <x:v>73.8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:19">
       <x:c r="E52" s="3" t="s">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="F52" s="4" t="n">
         <x:v>66.6</x:v>
@@ -3050,10 +3200,13 @@
       <x:c r="R52" s="4" t="n">
         <x:v>64.8</x:v>
       </x:c>
-    </x:row>
-    <x:row r="53" spans="1:18">
+      <x:c r="S52" s="4" t="n">
+        <x:v>67</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:19">
       <x:c r="E53" s="3" t="s">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="F53" s="4" t="n">
         <x:v>76</x:v>
@@ -3094,10 +3247,13 @@
       <x:c r="R53" s="4" t="n">
         <x:v>74.6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="54" spans="1:18">
+      <x:c r="S53" s="4" t="n">
+        <x:v>76.8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:19">
       <x:c r="E54" s="3" t="s">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="F54" s="4" t="n">
         <x:v>70.6</x:v>
@@ -3138,10 +3294,13 @@
       <x:c r="R54" s="4" t="n">
         <x:v>71.9</x:v>
       </x:c>
-    </x:row>
-    <x:row r="55" spans="1:18">
+      <x:c r="S54" s="4" t="n">
+        <x:v>73.4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:19">
       <x:c r="E55" s="3" t="s">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="F55" s="4" t="n">
         <x:v>78.6</x:v>
@@ -3182,10 +3341,13 @@
       <x:c r="R55" s="4" t="n">
         <x:v>76.4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="56" spans="1:18">
+      <x:c r="S55" s="4" t="n">
+        <x:v>79</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:19">
       <x:c r="E56" s="3" t="s">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="F56" s="4" t="n">
         <x:v>74</x:v>
@@ -3226,10 +3388,13 @@
       <x:c r="R56" s="4" t="n">
         <x:v>72</x:v>
       </x:c>
-    </x:row>
-    <x:row r="57" spans="1:18">
+      <x:c r="S56" s="4" t="n">
+        <x:v>74.7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:19">
       <x:c r="E57" s="3" t="s">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="F57" s="4" t="n">
         <x:v>77.1</x:v>
@@ -3270,10 +3435,13 @@
       <x:c r="R57" s="4" t="n">
         <x:v>75.8</x:v>
       </x:c>
-    </x:row>
-    <x:row r="58" spans="1:18">
+      <x:c r="S57" s="4" t="n">
+        <x:v>78</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:19">
       <x:c r="E58" s="3" t="s">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="F58" s="4" t="n">
         <x:v>77.8</x:v>
@@ -3314,10 +3482,13 @@
       <x:c r="R58" s="4" t="n">
         <x:v>77.6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="59" spans="1:18">
+      <x:c r="S58" s="4" t="n">
+        <x:v>79.2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:19">
       <x:c r="E59" s="3" t="s">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F59" s="4" t="n">
         <x:v>71.8</x:v>
@@ -3358,10 +3529,13 @@
       <x:c r="R59" s="4" t="n">
         <x:v>71.5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="60" spans="1:18">
+      <x:c r="S59" s="4" t="n">
+        <x:v>73.6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:19">
       <x:c r="E60" s="3" t="s">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="F60" s="4" t="n">
         <x:v>75.7</x:v>
@@ -3402,10 +3576,13 @@
       <x:c r="R60" s="4" t="n">
         <x:v>73.8</x:v>
       </x:c>
-    </x:row>
-    <x:row r="61" spans="1:18">
+      <x:c r="S60" s="4" t="n">
+        <x:v>76.5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:19">
       <x:c r="E61" s="3" t="s">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="F61" s="4" t="n">
         <x:v>73.4</x:v>
@@ -3446,10 +3623,13 @@
       <x:c r="R61" s="4" t="n">
         <x:v>71.2</x:v>
       </x:c>
-    </x:row>
-    <x:row r="62" spans="1:18">
+      <x:c r="S61" s="4" t="n">
+        <x:v>74.2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:19">
       <x:c r="E62" s="3" t="s">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="F62" s="4" t="n">
         <x:v>76</x:v>
@@ -3490,10 +3670,13 @@
       <x:c r="R62" s="4" t="n">
         <x:v>74.5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="63" spans="1:18">
+      <x:c r="S62" s="4" t="n">
+        <x:v>76.7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:19">
       <x:c r="E63" s="3" t="s">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="F63" s="4" t="n">
         <x:v>75.7</x:v>
@@ -3534,10 +3717,13 @@
       <x:c r="R63" s="4" t="n">
         <x:v>73.7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="64" spans="1:18">
+      <x:c r="S63" s="4" t="n">
+        <x:v>76.3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" spans="1:19">
       <x:c r="E64" s="3" t="s">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="F64" s="4" t="n">
         <x:v>76</x:v>
@@ -3578,10 +3764,13 @@
       <x:c r="R64" s="4" t="n">
         <x:v>74.6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="65" spans="1:18">
+      <x:c r="S64" s="4" t="n">
+        <x:v>77.2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" spans="1:19">
       <x:c r="E65" s="3" t="s">
-        <x:v>79</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="F65" s="4" t="n">
         <x:v>69</x:v>
@@ -3622,10 +3811,13 @@
       <x:c r="R65" s="4" t="n">
         <x:v>68.5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="66" spans="1:18">
+      <x:c r="S65" s="4" t="n">
+        <x:v>70.4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66" spans="1:19">
       <x:c r="E66" s="3" t="s">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="F66" s="4" t="n">
         <x:v>77.7</x:v>
@@ -3666,10 +3858,13 @@
       <x:c r="R66" s="4" t="n">
         <x:v>77.7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="67" spans="1:18">
+      <x:c r="S66" s="4" t="n">
+        <x:v>80.2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:19">
       <x:c r="E67" s="3" t="s">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="F67" s="4" t="n">
         <x:v>76.5</x:v>
@@ -3710,10 +3905,13 @@
       <x:c r="R67" s="4" t="n">
         <x:v>74.2</x:v>
       </x:c>
-    </x:row>
-    <x:row r="68" spans="1:18">
+      <x:c r="S67" s="4" t="n">
+        <x:v>76.4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:19">
       <x:c r="E68" s="3" t="s">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="F68" s="4" t="n">
         <x:v>73.9</x:v>
@@ -3754,10 +3952,13 @@
       <x:c r="R68" s="4" t="n">
         <x:v>71.2</x:v>
       </x:c>
-    </x:row>
-    <x:row r="69" spans="1:18">
+      <x:c r="S68" s="4" t="n">
+        <x:v>73.9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69" spans="1:19">
       <x:c r="E69" s="3" t="s">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="F69" s="4" t="n">
         <x:v>71.6</x:v>
@@ -3798,10 +3999,13 @@
       <x:c r="R69" s="4" t="n">
         <x:v>68.6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="70" spans="1:18">
+      <x:c r="S69" s="4" t="n">
+        <x:v>72.2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:19">
       <x:c r="E70" s="3" t="s">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="F70" s="4" t="n">
         <x:v>71.9</x:v>
@@ -3842,10 +4046,13 @@
       <x:c r="R70" s="4" t="n">
         <x:v>70.5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="71" spans="1:18">
+      <x:c r="S70" s="4" t="n">
+        <x:v>73.5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" spans="1:19">
       <x:c r="E71" s="3" t="s">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="F71" s="4" t="n">
         <x:v>68.4</x:v>
@@ -3886,10 +4093,13 @@
       <x:c r="R71" s="4" t="n">
         <x:v>69.7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="72" spans="1:18">
+      <x:c r="S71" s="4" t="n">
+        <x:v>71.6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72" spans="1:19">
       <x:c r="E72" s="3" t="s">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F72" s="4" t="n">
         <x:v>77.2</x:v>
@@ -3930,10 +4140,13 @@
       <x:c r="R72" s="4" t="n">
         <x:v>75.5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="73" spans="1:18">
+      <x:c r="S72" s="4" t="n">
+        <x:v>78</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73" spans="1:19">
       <x:c r="E73" s="3" t="s">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="F73" s="4" t="n">
         <x:v>80.1</x:v>
@@ -3974,10 +4187,13 @@
       <x:c r="R73" s="4" t="n">
         <x:v>76.7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="74" spans="1:18">
+      <x:c r="S73" s="4" t="n">
+        <x:v>79.7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74" spans="1:19">
       <x:c r="E74" s="3" t="s">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="F74" s="4" t="n">
         <x:v>75</x:v>
@@ -4018,10 +4234,13 @@
       <x:c r="R74" s="4" t="n">
         <x:v>75.2</x:v>
       </x:c>
-    </x:row>
-    <x:row r="75" spans="1:18">
+      <x:c r="S74" s="4" t="n">
+        <x:v>77.7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75" spans="1:19">
       <x:c r="E75" s="3" t="s">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="F75" s="4" t="n">
         <x:v>74.7</x:v>
@@ -4062,10 +4281,13 @@
       <x:c r="R75" s="4" t="n">
         <x:v>75.8</x:v>
       </x:c>
-    </x:row>
-    <x:row r="76" spans="1:18">
+      <x:c r="S75" s="4" t="n">
+        <x:v>77.8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="76" spans="1:19">
       <x:c r="E76" s="3" t="s">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F76" s="4" t="n">
         <x:v>75.9</x:v>
@@ -4106,10 +4328,13 @@
       <x:c r="R76" s="4" t="n">
         <x:v>73.3</x:v>
       </x:c>
-    </x:row>
-    <x:row r="77" spans="1:18">
+      <x:c r="S76" s="4" t="n">
+        <x:v>76.3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="77" spans="1:19">
       <x:c r="E77" s="3" t="s">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="F77" s="4" t="n">
         <x:v>76.8</x:v>
@@ -4150,10 +4375,13 @@
       <x:c r="R77" s="4" t="n">
         <x:v>73.9</x:v>
       </x:c>
-    </x:row>
-    <x:row r="78" spans="1:18">
+      <x:c r="S77" s="4" t="n">
+        <x:v>76.6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="78" spans="1:19">
       <x:c r="E78" s="3" t="s">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="F78" s="4" t="n">
         <x:v>78.7</x:v>
@@ -4194,10 +4422,13 @@
       <x:c r="R78" s="4" t="n">
         <x:v>76.5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="79" spans="1:18">
+      <x:c r="S78" s="4" t="n">
+        <x:v>79.3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79" spans="1:19">
       <x:c r="E79" s="3" t="s">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F79" s="4" t="n">
         <x:v>75.1</x:v>
@@ -4238,10 +4469,13 @@
       <x:c r="R79" s="4" t="n">
         <x:v>73</x:v>
       </x:c>
-    </x:row>
-    <x:row r="80" spans="1:18">
+      <x:c r="S79" s="4" t="n">
+        <x:v>75.5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="80" spans="1:19">
       <x:c r="E80" s="3" t="s">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="F80" s="4" t="n">
         <x:v>75.7</x:v>
@@ -4282,10 +4516,13 @@
       <x:c r="R80" s="4" t="n">
         <x:v>73.8</x:v>
       </x:c>
-    </x:row>
-    <x:row r="81" spans="1:18">
+      <x:c r="S80" s="4" t="n">
+        <x:v>75.8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="81" spans="1:19">
       <x:c r="E81" s="3" t="s">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="F81" s="4" t="n">
         <x:v>80.9</x:v>
@@ -4326,10 +4563,13 @@
       <x:c r="R81" s="4" t="n">
         <x:v>78.6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="82" spans="1:18">
+      <x:c r="S81" s="4" t="n">
+        <x:v>80.4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="82" spans="1:19">
       <x:c r="E82" s="3" t="s">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="F82" s="4" t="n">
         <x:v>79.6</x:v>
@@ -4370,10 +4610,13 @@
       <x:c r="R82" s="4" t="n">
         <x:v>78.7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="83" spans="1:18">
+      <x:c r="S82" s="4" t="n">
+        <x:v>81.1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="83" spans="1:19">
       <x:c r="E83" s="3" t="s">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="F83" s="4" t="n">
         <x:v>79.2</x:v>
@@ -4414,10 +4657,13 @@
       <x:c r="R83" s="4" t="n">
         <x:v>77.1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="84" spans="1:18">
+      <x:c r="S83" s="4" t="n">
+        <x:v>79.5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="84" spans="1:19">
       <x:c r="E84" s="3" t="s">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="F84" s="4" t="n">
         <x:v>74.6</x:v>
@@ -4458,10 +4704,13 @@
       <x:c r="R84" s="4" t="n">
         <x:v>73.8</x:v>
       </x:c>
-    </x:row>
-    <x:row r="85" spans="1:18">
+      <x:c r="S84" s="4" t="n">
+        <x:v>75.5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="85" spans="1:19">
       <x:c r="E85" s="3" t="s">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F85" s="4" t="n">
         <x:v>77</x:v>
@@ -4502,10 +4751,13 @@
       <x:c r="R85" s="4" t="n">
         <x:v>75</x:v>
       </x:c>
-    </x:row>
-    <x:row r="86" spans="1:18">
+      <x:c r="S85" s="4" t="n">
+        <x:v>77.6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="86" spans="1:19">
       <x:c r="E86" s="3" t="s">
-        <x:v>100</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F86" s="4" t="n">
         <x:v>76.2</x:v>
@@ -4546,10 +4798,13 @@
       <x:c r="R86" s="4" t="n">
         <x:v>74.3</x:v>
       </x:c>
-    </x:row>
-    <x:row r="87" spans="1:18">
+      <x:c r="S86" s="4" t="n">
+        <x:v>77</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="87" spans="1:19">
       <x:c r="E87" s="3" t="s">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F87" s="4" t="n">
         <x:v>81.8</x:v>
@@ -4590,10 +4845,13 @@
       <x:c r="R87" s="4" t="n">
         <x:v>80.7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="88" spans="1:18">
+      <x:c r="S87" s="4" t="n">
+        <x:v>82.6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="88" spans="1:19">
       <x:c r="E88" s="3" t="s">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="F88" s="4" t="n">
         <x:v>82.3</x:v>
@@ -4634,10 +4892,13 @@
       <x:c r="R88" s="4" t="n">
         <x:v>80.1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="89" spans="1:18">
+      <x:c r="S88" s="4" t="n">
+        <x:v>82.2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="89" spans="1:19">
       <x:c r="E89" s="3" t="s">
-        <x:v>103</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="F89" s="4" t="n">
         <x:v>76.6</x:v>
@@ -4678,10 +4939,13 @@
       <x:c r="R89" s="4" t="n">
         <x:v>75.6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="90" spans="1:18">
+      <x:c r="S89" s="4" t="n">
+        <x:v>78.2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="90" spans="1:19">
       <x:c r="E90" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="F90" s="4" t="n">
         <x:v>74.4</x:v>
@@ -4722,10 +4986,13 @@
       <x:c r="R90" s="4" t="n">
         <x:v>72.7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="91" spans="1:18">
+      <x:c r="S90" s="4" t="n">
+        <x:v>74.4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="91" spans="1:19">
       <x:c r="E91" s="3" t="s">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="F91" s="4" t="n">
         <x:v>79</x:v>
@@ -4766,10 +5033,13 @@
       <x:c r="R91" s="4" t="n">
         <x:v>77.9</x:v>
       </x:c>
-    </x:row>
-    <x:row r="92" spans="1:18">
+      <x:c r="S91" s="4" t="n">
+        <x:v>80</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="92" spans="1:19">
       <x:c r="E92" s="3" t="s">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="F92" s="4" t="n">
         <x:v>76.3</x:v>
@@ -4810,10 +5080,13 @@
       <x:c r="R92" s="4" t="n">
         <x:v>73.9</x:v>
       </x:c>
-    </x:row>
-    <x:row r="93" spans="1:18">
+      <x:c r="S92" s="4" t="n">
+        <x:v>76.4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="93" spans="1:19">
       <x:c r="E93" s="3" t="s">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="F93" s="4" t="n">
         <x:v>70.8</x:v>
@@ -4854,10 +5127,13 @@
       <x:c r="R93" s="4" t="n">
         <x:v>74.3</x:v>
       </x:c>
-    </x:row>
-    <x:row r="94" spans="1:18">
+      <x:c r="S93" s="4" t="n">
+        <x:v>76.2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="94" spans="1:19">
       <x:c r="E94" s="3" t="s">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="F94" s="4" t="n">
         <x:v>79.5</x:v>
@@ -4898,10 +5174,13 @@
       <x:c r="R94" s="4" t="n">
         <x:v>78</x:v>
       </x:c>
-    </x:row>
-    <x:row r="95" spans="1:18">
+      <x:c r="S94" s="4" t="n">
+        <x:v>80.3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="95" spans="1:19">
       <x:c r="E95" s="3" t="s">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="F95" s="4" t="n">
         <x:v>81.4</x:v>
@@ -4942,10 +5221,13 @@
       <x:c r="R95" s="4" t="n">
         <x:v>80.7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="96" spans="1:18">
+      <x:c r="S95" s="4" t="n">
+        <x:v>82.8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96" spans="1:19">
       <x:c r="E96" s="3" t="s">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="F96" s="4" t="n">
         <x:v>76.6</x:v>
@@ -4986,10 +5268,13 @@
       <x:c r="R96" s="4" t="n">
         <x:v>76.5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="97" spans="1:18">
+      <x:c r="S96" s="4" t="n">
+        <x:v>78.5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97" spans="1:19">
       <x:c r="E97" s="3" t="s">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="F97" s="4" t="n">
         <x:v>72.6</x:v>
@@ -5030,10 +5315,13 @@
       <x:c r="R97" s="4" t="n">
         <x:v>70.5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="98" spans="1:18">
+      <x:c r="S97" s="4" t="n">
+        <x:v>73.7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="98" spans="1:19">
       <x:c r="E98" s="3" t="s">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="F98" s="4" t="n">
         <x:v>78.8</x:v>
@@ -5074,10 +5362,13 @@
       <x:c r="R98" s="4" t="n">
         <x:v>76.7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="99" spans="1:18">
+      <x:c r="S98" s="4" t="n">
+        <x:v>79.1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99" spans="1:19">
       <x:c r="E99" s="3" t="s">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="F99" s="4" t="n">
         <x:v>78.6</x:v>
@@ -5118,10 +5409,13 @@
       <x:c r="R99" s="4" t="n">
         <x:v>77</x:v>
       </x:c>
-    </x:row>
-    <x:row r="100" spans="1:18">
+      <x:c r="S99" s="4" t="n">
+        <x:v>79.7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="100" spans="1:19">
       <x:c r="E100" s="3" t="s">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="F100" s="4" t="n">
         <x:v>79.2</x:v>
@@ -5162,10 +5456,13 @@
       <x:c r="R100" s="4" t="n">
         <x:v>78.4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="101" spans="1:18">
+      <x:c r="S100" s="4" t="n">
+        <x:v>80.1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="101" spans="1:19">
       <x:c r="E101" s="3" t="s">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="F101" s="4" t="n">
         <x:v>79</x:v>
@@ -5206,10 +5503,13 @@
       <x:c r="R101" s="4" t="n">
         <x:v>75.5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="102" spans="1:18">
+      <x:c r="S101" s="4" t="n">
+        <x:v>78.2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="102" spans="1:19">
       <x:c r="E102" s="3" t="s">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="F102" s="4" t="n">
         <x:v>78.4</x:v>
@@ -5250,10 +5550,13 @@
       <x:c r="R102" s="4" t="n">
         <x:v>77.5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="103" spans="1:18">
+      <x:c r="S102" s="4" t="n">
+        <x:v>79.4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="103" spans="1:19">
       <x:c r="E103" s="3" t="s">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="F103" s="4" t="n">
         <x:v>80.8</x:v>
@@ -5294,10 +5597,13 @@
       <x:c r="R103" s="4" t="n">
         <x:v>78.3</x:v>
       </x:c>
-    </x:row>
-    <x:row r="104" spans="1:18">
+      <x:c r="S103" s="4" t="n">
+        <x:v>80.4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="104" spans="1:19">
       <x:c r="E104" s="3" t="s">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="F104" s="4" t="n">
         <x:v>76.5</x:v>
@@ -5338,10 +5644,13 @@
       <x:c r="R104" s="4" t="n">
         <x:v>75.4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="105" spans="1:18">
+      <x:c r="S104" s="4" t="n">
+        <x:v>77.9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="105" spans="1:19">
       <x:c r="E105" s="3" t="s">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="F105" s="4" t="n">
         <x:v>76.4</x:v>
@@ -5382,10 +5691,13 @@
       <x:c r="R105" s="4" t="n">
         <x:v>74.2</x:v>
       </x:c>
-    </x:row>
-    <x:row r="106" spans="1:18">
+      <x:c r="S105" s="4" t="n">
+        <x:v>76.8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="106" spans="1:19">
       <x:c r="E106" s="3" t="s">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F106" s="4" t="n">
         <x:v>79.4</x:v>
@@ -5426,10 +5738,13 @@
       <x:c r="R106" s="4" t="n">
         <x:v>76.1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="107" spans="1:18">
+      <x:c r="S106" s="4" t="n">
+        <x:v>78.3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="107" spans="1:19">
       <x:c r="E107" s="3" t="s">
-        <x:v>121</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="F107" s="4" t="n">
         <x:v>75.2</x:v>
@@ -5470,10 +5785,13 @@
       <x:c r="R107" s="4" t="n">
         <x:v>73.3</x:v>
       </x:c>
-    </x:row>
-    <x:row r="108" spans="1:18">
+      <x:c r="S107" s="4" t="n">
+        <x:v>76.1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="108" spans="1:19">
       <x:c r="E108" s="3" t="s">
-        <x:v>122</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="F108" s="4" t="n">
         <x:v>75.2</x:v>
@@ -5514,10 +5832,13 @@
       <x:c r="R108" s="4" t="n">
         <x:v>73.3</x:v>
       </x:c>
-    </x:row>
-    <x:row r="109" spans="1:18">
+      <x:c r="S108" s="4" t="n">
+        <x:v>76.1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="109" spans="1:19">
       <x:c r="E109" s="3" t="s">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="F109" s="4" t="n">
         <x:v>76.2</x:v>
@@ -5558,10 +5879,13 @@
       <x:c r="R109" s="4" t="n">
         <x:v>75.1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="110" spans="1:18">
+      <x:c r="S109" s="4" t="n">
+        <x:v>78.2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="110" spans="1:19">
       <x:c r="E110" s="3" t="s">
-        <x:v>124</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="F110" s="4" t="n">
         <x:v>74.4</x:v>
@@ -5602,10 +5926,13 @@
       <x:c r="R110" s="4" t="n">
         <x:v>72.6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="111" spans="1:18">
+      <x:c r="S110" s="4" t="n">
+        <x:v>75.2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="111" spans="1:19">
       <x:c r="E111" s="3" t="s">
-        <x:v>125</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="F111" s="4" t="n">
         <x:v>75.5</x:v>
@@ -5646,10 +5973,13 @@
       <x:c r="R111" s="4" t="n">
         <x:v>73.9</x:v>
       </x:c>
-    </x:row>
-    <x:row r="112" spans="1:18">
+      <x:c r="S111" s="4" t="n">
+        <x:v>76.3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="112" spans="1:19">
       <x:c r="E112" s="3" t="s">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="F112" s="4" t="n">
         <x:v>76.3</x:v>
@@ -5690,10 +6020,13 @@
       <x:c r="R112" s="4" t="n">
         <x:v>75</x:v>
       </x:c>
-    </x:row>
-    <x:row r="113" spans="1:18">
+      <x:c r="S112" s="4" t="n">
+        <x:v>77.6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="113" spans="1:19">
       <x:c r="E113" s="3" t="s">
-        <x:v>127</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="F113" s="4" t="n">
         <x:v>73.1</x:v>
@@ -5734,10 +6067,13 @@
       <x:c r="R113" s="4" t="n">
         <x:v>74.6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="114" spans="1:18">
+      <x:c r="S113" s="4" t="n">
+        <x:v>74.3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="114" spans="1:19">
       <x:c r="E114" s="3" t="s">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="F114" s="4" t="n">
         <x:v>77.1</x:v>
@@ -5778,10 +6114,13 @@
       <x:c r="R114" s="4" t="n">
         <x:v>74.7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="115" spans="1:18">
+      <x:c r="S114" s="4" t="n">
+        <x:v>77.3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="115" spans="1:19">
       <x:c r="E115" s="3" t="s">
-        <x:v>129</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="F115" s="4" t="n">
         <x:v>73.1</x:v>
@@ -5822,10 +6161,13 @@
       <x:c r="R115" s="4" t="n">
         <x:v>74.3</x:v>
       </x:c>
-    </x:row>
-    <x:row r="116" spans="1:18">
+      <x:c r="S115" s="4" t="n">
+        <x:v>76.2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="116" spans="1:19">
       <x:c r="E116" s="3" t="s">
-        <x:v>130</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="F116" s="4" t="n">
         <x:v>81</x:v>
@@ -5866,10 +6208,13 @@
       <x:c r="R116" s="4" t="n">
         <x:v>80.1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="117" spans="1:18">
+      <x:c r="S116" s="4" t="n">
+        <x:v>82.5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="117" spans="1:19">
       <x:c r="E117" s="3" t="s">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F117" s="4" t="n">
         <x:v>76.9</x:v>
@@ -5910,10 +6255,13 @@
       <x:c r="R117" s="4" t="n">
         <x:v>75.7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="118" spans="1:18">
+      <x:c r="S117" s="4" t="n">
+        <x:v>77.9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="118" spans="1:19">
       <x:c r="E118" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="F118" s="4" t="n">
         <x:v>76.9</x:v>
@@ -5954,10 +6302,13 @@
       <x:c r="R118" s="4" t="n">
         <x:v>74.8</x:v>
       </x:c>
-    </x:row>
-    <x:row r="119" spans="1:18">
+      <x:c r="S118" s="4" t="n">
+        <x:v>77.1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="119" spans="1:19">
       <x:c r="E119" s="3" t="s">
-        <x:v>133</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="F119" s="4" t="n">
         <x:v>73.2</x:v>
@@ -5997,6 +6348,9 @@
       </x:c>
       <x:c r="R119" s="4" t="n">
         <x:v>71</x:v>
+      </x:c>
+      <x:c r="S119" s="4" t="n">
+        <x:v>74.3</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>